<commit_message>
UPDATE Terakhir BKK (Semua fitur done) - 11/11/2019
</commit_message>
<xml_diff>
--- a/assets/excel/import_data.xlsx
+++ b/assets/excel/import_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
   <si>
     <t>NISN</t>
   </si>
@@ -68,41 +68,86 @@
     <t>Nama Lengkap</t>
   </si>
   <si>
-    <t>asdad</t>
+    <t>Alumni 2</t>
+  </si>
+  <si>
+    <t>Alumni 3</t>
+  </si>
+  <si>
+    <t>Alumni 4</t>
+  </si>
+  <si>
+    <t>Alumni 5</t>
+  </si>
+  <si>
+    <t>Alumni 6</t>
+  </si>
+  <si>
+    <t>P</t>
   </si>
   <si>
     <t>L</t>
   </si>
   <si>
-    <t>asdasf</t>
-  </si>
-  <si>
-    <t>dasdad</t>
-  </si>
-  <si>
-    <t>asdasd</t>
-  </si>
-  <si>
-    <t>calenger747@gmail.com</t>
-  </si>
-  <si>
-    <t>Rekayasa Perangkat Lunak</t>
+    <t>Depok</t>
+  </si>
+  <si>
+    <t>Bogor</t>
+  </si>
+  <si>
+    <t>Bekasi</t>
+  </si>
+  <si>
+    <t>Tangerang</t>
+  </si>
+  <si>
+    <t>Bandung</t>
+  </si>
+  <si>
+    <t>Jakarta</t>
+  </si>
+  <si>
+    <t>alumni2@gmail.com</t>
+  </si>
+  <si>
+    <t>alumni3@gmail.com</t>
+  </si>
+  <si>
+    <t>alumni4@gmail.com</t>
+  </si>
+  <si>
+    <t>alumni5@gmail.com</t>
+  </si>
+  <si>
+    <t>alumni6@gmail.com</t>
+  </si>
+  <si>
+    <t>Teknologi Informasi dan Komunikasi</t>
+  </si>
+  <si>
+    <t>Belum Bekerja</t>
+  </si>
+  <si>
+    <t>Wiraswasta</t>
+  </si>
+  <si>
+    <t>Kuliah</t>
   </si>
   <si>
     <t>Bekerja</t>
   </si>
   <si>
-    <t>abc</t>
-  </si>
-  <si>
-    <t>depok</t>
+    <t>Perusahaan B</t>
+  </si>
+  <si>
+    <t>Perusahaan C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,6 +162,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -140,13 +190,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -154,74 +205,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -238,10 +221,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="14181B"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="F0F1F2"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -520,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,7 +520,7 @@
     <col min="7" max="7" width="41.5703125" customWidth="1"/>
     <col min="8" max="8" width="24.28515625" customWidth="1"/>
     <col min="9" max="9" width="21.140625" customWidth="1"/>
-    <col min="10" max="10" width="26.140625" customWidth="1"/>
+    <col min="10" max="10" width="36.5703125" customWidth="1"/>
     <col min="11" max="11" width="18.28515625" customWidth="1"/>
     <col min="12" max="12" width="31.28515625" customWidth="1"/>
     <col min="13" max="13" width="21.42578125" customWidth="1"/>
@@ -594,56 +577,225 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>411</v>
+        <v>23456</v>
       </c>
       <c r="B2">
-        <v>1414</v>
+        <v>23456</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="F2" s="2">
-        <v>43748</v>
+        <v>36811</v>
       </c>
       <c r="G2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" t="s">
-        <v>19</v>
+        <v>22</v>
+      </c>
+      <c r="H2">
+        <v>23456</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" t="s">
-        <v>21</v>
+        <v>28</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="K2">
         <v>2018</v>
       </c>
       <c r="L2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>23457</v>
+      </c>
+      <c r="B3">
+        <v>23457</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="2">
+        <v>36526</v>
+      </c>
+      <c r="G3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3">
+        <v>23457</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3">
+        <v>2018</v>
+      </c>
+      <c r="L3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>23458</v>
+      </c>
+      <c r="B4">
+        <v>23458</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="2">
+        <v>36241</v>
+      </c>
+      <c r="G4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4">
+        <v>23458</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K4">
+        <v>2017</v>
+      </c>
+      <c r="L4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>23459</v>
+      </c>
+      <c r="B5">
+        <v>23459</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="2">
+        <v>35956</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5">
+        <v>23459</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K5">
+        <v>2016</v>
+      </c>
+      <c r="L5" t="s">
+        <v>37</v>
+      </c>
+      <c r="M5" t="s">
+        <v>38</v>
+      </c>
+      <c r="N5" t="s">
         <v>22</v>
       </c>
-      <c r="M2" t="s">
-        <v>23</v>
-      </c>
-      <c r="N2" t="s">
-        <v>24</v>
-      </c>
-      <c r="O2">
-        <v>8918311</v>
+      <c r="O5">
+        <v>2345677</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>23460</v>
+      </c>
+      <c r="B6">
+        <v>23460</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="2">
+        <v>35671</v>
+      </c>
+      <c r="G6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6">
+        <v>23460</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K6">
+        <v>2015</v>
+      </c>
+      <c r="L6" t="s">
+        <v>37</v>
+      </c>
+      <c r="M6" t="s">
+        <v>39</v>
+      </c>
+      <c r="N6" t="s">
+        <v>22</v>
+      </c>
+      <c r="O6">
+        <v>123121213</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Belum Bekerja" sqref="L2"/>
+  </dataValidations>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1"/>
+    <hyperlink ref="I3" r:id="rId2"/>
+    <hyperlink ref="I4" r:id="rId3"/>
+    <hyperlink ref="I5" r:id="rId4"/>
+    <hyperlink ref="I6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 

</xml_diff>